<commit_message>
FreeCodeCamp article links added.
</commit_message>
<xml_diff>
--- a/Chrome Tab.xlsx
+++ b/Chrome Tab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B11EA0-36A3-4EC9-BB2C-5F8BC8AC77B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C174A-4149-4AC3-8AAD-9B4F3BB474F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" firstSheet="2" activeTab="8" xr2:uid="{6E38DE2F-54D6-4076-A0D5-B44B8C4EE2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" firstSheet="2" activeTab="10" xr2:uid="{6E38DE2F-54D6-4076-A0D5-B44B8C4EE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="343">
   <si>
     <t>https://www.youtube.com/playlist?list=PLU_sdQYzUj2keVENTP0a5rdykRSgg9Wp-</t>
   </si>
@@ -1020,6 +1020,51 @@
   </si>
   <si>
     <t>Udemy - Beginner Guide to Android app Development</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/develop-a-covid-19-live-web-app-with-python-django/</t>
+  </si>
+  <si>
+    <t>Udemy - Django Covid19 app</t>
+  </si>
+  <si>
+    <t>https://careers.google.com/jobs/results/?degree=BACHELORS&amp;q=&amp;skills=Programming</t>
+  </si>
+  <si>
+    <t>https://amazonvirtualhiring.hirepro.in/registration/incta/ju0f4/openings/</t>
+  </si>
+  <si>
+    <t>Google Jobs</t>
+  </si>
+  <si>
+    <t>Amazon Jobs</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp - Build React Hooks</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/how-to-create-react-hooks/</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp - React Basics</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/react-testing-library-tutorial-javascript-example-code/</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp - Testing in React</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/git-cheat-sheet/</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp - Git Commands</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/how-classes-work-in-cplusplus/</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp - How Classes Works</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB7272F-DEE2-4241-B8D3-3016BFCC270D}">
-  <dimension ref="B2:C56"/>
+  <dimension ref="B2:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1694,6 +1739,30 @@
       </c>
       <c r="C56" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" t="s">
+        <v>332</v>
+      </c>
+      <c r="C58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>333</v>
+      </c>
+      <c r="C60" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -1744,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384A864D-AA69-4DD4-861A-5F6B2AE785A5}">
-  <dimension ref="B3:C13"/>
+  <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1789,6 +1858,14 @@
         <v>123</v>
       </c>
     </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1796,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD04119-EB50-4C00-81B8-A3CABB0D7B1C}">
-  <dimension ref="B3:C41"/>
+  <dimension ref="B3:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1966,6 +2043,14 @@
       </c>
       <c r="C41" t="s">
         <v>304</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>329</v>
+      </c>
+      <c r="C43" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2684,16 +2769,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2E5E96-72C6-4E09-852A-C11493349E62}">
-  <dimension ref="B3:C33"/>
+  <dimension ref="B3:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="70.88671875" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
@@ -2822,6 +2907,30 @@
       </c>
       <c r="C33" s="11" t="s">
         <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>336</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C37" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>338</v>
+      </c>
+      <c r="C39" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2833,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A308F767-9432-4FF8-B757-42F2157A09C3}">
   <dimension ref="B2:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DataCamp python course added.
</commit_message>
<xml_diff>
--- a/Chrome Tab.xlsx
+++ b/Chrome Tab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C174A-4149-4AC3-8AAD-9B4F3BB474F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E60AAA-71B8-4408-A38A-759FD38AEDA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" firstSheet="2" activeTab="10" xr2:uid="{6E38DE2F-54D6-4076-A0D5-B44B8C4EE2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" firstSheet="2" activeTab="11" xr2:uid="{6E38DE2F-54D6-4076-A0D5-B44B8C4EE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="347">
   <si>
     <t>https://www.youtube.com/playlist?list=PLU_sdQYzUj2keVENTP0a5rdykRSgg9Wp-</t>
   </si>
@@ -1065,6 +1065,18 @@
   </si>
   <si>
     <t>FreeCodeCamp - How Classes Works</t>
+  </si>
+  <si>
+    <t>https://learn.datacamp.com/courses/introduction-to-python-for-finance</t>
+  </si>
+  <si>
+    <t>DataCamp</t>
+  </si>
+  <si>
+    <t>https://learn.datacamp.com/courses/developing-python-packages</t>
+  </si>
+  <si>
+    <t>https://learn.datacamp.com/courses/writing-functions-in-python</t>
   </si>
 </sst>
 </file>
@@ -1815,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384A864D-AA69-4DD4-861A-5F6B2AE785A5}">
   <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1873,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD04119-EB50-4C00-81B8-A3CABB0D7B1C}">
-  <dimension ref="B3:C43"/>
+  <dimension ref="B3:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2051,6 +2063,30 @@
       </c>
       <c r="C43" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Android resources by google added.
</commit_message>
<xml_diff>
--- a/Chrome Tab.xlsx
+++ b/Chrome Tab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB64D7E1-6C1D-413D-99CF-5785F17BC5F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F27294-6472-4ABA-A533-871CD29F8608}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" firstSheet="2" activeTab="8" xr2:uid="{6E38DE2F-54D6-4076-A0D5-B44B8C4EE2D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="355">
   <si>
     <t>https://www.youtube.com/playlist?list=PLU_sdQYzUj2keVENTP0a5rdykRSgg9Wp-</t>
   </si>
@@ -1077,6 +1077,30 @@
   </si>
   <si>
     <t>https://learn.datacamp.com/courses/writing-functions-in-python</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/studio/</t>
+  </si>
+  <si>
+    <t>Android Studio</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/kotlin</t>
+  </si>
+  <si>
+    <t>Android Kotlin</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/courses/android-basics-kotlin/course</t>
+  </si>
+  <si>
+    <t>Android Google Kotlin</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/</t>
+  </si>
+  <si>
+    <t>Android Google Developer</t>
   </si>
 </sst>
 </file>
@@ -2976,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A308F767-9432-4FF8-B757-42F2157A09C3}">
-  <dimension ref="B2:C49"/>
+  <dimension ref="B2:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3183,6 +3207,38 @@
         <v>326</v>
       </c>
     </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>348</v>
+      </c>
+      <c r="C51" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>350</v>
+      </c>
+      <c r="C53" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" t="s">
+        <v>352</v>
+      </c>
+      <c r="C55" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>354</v>
+      </c>
+      <c r="C57" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>